<commit_message>
Added code to almost all Controllers Update EntityFramework.6.1.3
</commit_message>
<xml_diff>
--- a/DB/Названия таблиц.xlsx
+++ b/DB/Названия таблиц.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>citiruemost_publikaciy_pps_vuza_rus_uz</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>nalichie_informacii_o_vuze_v_internete</t>
-  </si>
-  <si>
-    <t>osnashennost_laboratornim_oborudovaniem</t>
   </si>
   <si>
     <t>nalichie_multimedia_v_auditorii</t>
@@ -109,12 +106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -448,7 +452,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,10 +569,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -597,11 +601,11 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
-        <v>21</v>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +613,7 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>